<commit_message>
add fields for start and end date of patient recruitment, all data currently missing
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/personal/health_ai/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/health-ai-performance/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D8DCA4-39B9-9D4E-B577-EAD446CEC2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6E1753-6097-8648-84DF-7FB55F9425CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="272">
   <si>
     <t>Text</t>
   </si>
@@ -836,6 +836,24 @@
   </si>
   <si>
     <t>Used, with corresponding online dataset to identify select AI/ML algorithms authorized by the US FDA (see also https://ericwu09.github.io/medical-ai-evaluation/#)</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
+    <t>The date that data collection and/or patient enrollment ended in order to calculate the metric, if any is specified</t>
+  </si>
+  <si>
+    <t>The date that data collection and/or patient enrollment started in order to calculate the metric, if any is specified</t>
   </si>
 </sst>
 </file>
@@ -1042,6 +1060,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1050,12 +1074,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1300,26 +1318,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="3" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
@@ -1328,13 +1346,13 @@
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:22" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:22" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
@@ -3616,10 +3634,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U1016"/>
+  <dimension ref="A1:U1018"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3639,14 +3657,14 @@
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:21" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="1:21" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -4418,11 +4436,17 @@
         <v>170</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+        <v>266</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -4445,11 +4469,17 @@
         <v>170</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+        <v>267</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>1</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -4472,7 +4502,7 @@
         <v>170</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -4499,7 +4529,7 @@
         <v>170</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -4526,7 +4556,7 @@
         <v>170</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -4553,7 +4583,7 @@
         <v>170</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -4580,7 +4610,7 @@
         <v>170</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -4603,8 +4633,12 @@
       <c r="U33" s="2"/>
     </row>
     <row r="34" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="A34" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>183</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -4626,8 +4660,12 @@
       <c r="U34" s="2"/>
     </row>
     <row r="35" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="A35" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>186</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -4948,50 +4986,50 @@
       <c r="U48" s="2"/>
     </row>
     <row r="49" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
     </row>
     <row r="50" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
     </row>
     <row r="51" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
@@ -5384,7 +5422,7 @@
       <c r="T67" s="3"/>
       <c r="U67" s="3"/>
     </row>
-    <row r="68" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -5407,7 +5445,7 @@
       <c r="T68" s="3"/>
       <c r="U68" s="3"/>
     </row>
-    <row r="69" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -5430,8 +5468,52 @@
       <c r="T69" s="3"/>
       <c r="U69" s="3"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+    </row>
+    <row r="71" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3"/>
+      <c r="U71" s="3"/>
+    </row>
     <row r="72" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="73" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6377,6 +6459,8 @@
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:F2"/>
@@ -6412,13 +6496,13 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:19" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -8430,7 +8514,7 @@
   </sheetPr>
   <dimension ref="A1:R999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -8447,12 +8531,12 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:18" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3" spans="1:18" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -8584,10 +8668,10 @@
       <c r="A8" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="18" t="s">
         <v>264</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -10477,13 +10561,13 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:19" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">

</xml_diff>

<commit_message>
add rate ranges for studies that reported that info
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/health-ai-performance/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6E1753-6097-8648-84DF-7FB55F9425CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EAFDF4-0B66-D04D-982E-F1DE33250D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="275">
   <si>
     <t>Text</t>
   </si>
@@ -487,9 +487,6 @@
     <t>This data dictionary is intended to document the dataset(s) accessible at [internal use only]</t>
   </si>
   <si>
-    <t>The data dictionary was last updated on July 17, 2023</t>
-  </si>
-  <si>
     <t>Ad hoc</t>
   </si>
   <si>
@@ -685,9 +682,6 @@
     <t>Used to identify select AI/ML algorithms authorized by the US FDA</t>
   </si>
   <si>
-    <t>input_id</t>
-  </si>
-  <si>
     <t>FDA authorization pathway</t>
   </si>
   <si>
@@ -733,9 +727,6 @@
     <t>Still in progress, maintainer dropped as it can change over time and would need to be logged with a "freshness" date, didn't seem like a sufficiently valuable data point</t>
   </si>
   <si>
-    <t>Added additional field descriptions, dropped field "maintainer"</t>
-  </si>
-  <si>
     <t>References</t>
   </si>
   <si>
@@ -745,9 +736,6 @@
     <t>Added as documents within airtable</t>
   </si>
   <si>
-    <t>Input ID</t>
-  </si>
-  <si>
     <t>observations</t>
   </si>
   <si>
@@ -811,18 +799,9 @@
     <t>Observation name</t>
   </si>
   <si>
-    <t>A unique numeric ID for each observation or data type</t>
-  </si>
-  <si>
     <t>A name for each observation or data type</t>
   </si>
   <si>
-    <t>observation_id</t>
-  </si>
-  <si>
-    <t>Observation ID</t>
-  </si>
-  <si>
     <t>observation_description</t>
   </si>
   <si>
@@ -854,6 +833,36 @@
   </si>
   <si>
     <t>The date that data collection and/or patient enrollment started in order to calculate the metric, if any is specified</t>
+  </si>
+  <si>
+    <t>Added additional fields for descriptions, dropped field "maintainer"</t>
+  </si>
+  <si>
+    <t>Added additional fields for dates of study development, validation, or real-world use</t>
+  </si>
+  <si>
+    <t>May be useful in the future for tracking things like performance drift, at the very least, useful to assess recency of studies</t>
+  </si>
+  <si>
+    <t>In the case that specific dates are not reported (e.g., only year or only month and year), start dates are assumed to start on the first day of the month.</t>
+  </si>
+  <si>
+    <t>In the case that specific dates are not reported (e.g., only year or only month and year), end dates are assumed to start on the last day of the month.</t>
+  </si>
+  <si>
+    <t>Observation description</t>
+  </si>
+  <si>
+    <t>A description of how each observation was calculated, if available, this is often quoted directly from the referenced source</t>
+  </si>
+  <si>
+    <t>Algorithm metric ID</t>
+  </si>
+  <si>
+    <t>A unique ID for each metric reported for each algorithm</t>
+  </si>
+  <si>
+    <t>The data dictionary was last updated on September 24, 2023</t>
   </si>
 </sst>
 </file>
@@ -1304,8 +1313,8 @@
   </sheetPr>
   <dimension ref="A1:V1005"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1333,7 +1342,7 @@
     </row>
     <row r="3" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>149</v>
+        <v>274</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
@@ -1373,19 +1382,19 @@
     </row>
     <row r="7" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>168</v>
-      </c>
       <c r="D7" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1407,19 +1416,19 @@
     </row>
     <row r="8" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>204</v>
-      </c>
       <c r="D8" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1441,19 +1450,19 @@
     </row>
     <row r="9" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>206</v>
-      </c>
       <c r="D9" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1475,19 +1484,19 @@
     </row>
     <row r="10" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1509,19 +1518,19 @@
     </row>
     <row r="11" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>173</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -3634,10 +3643,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U1018"/>
+  <dimension ref="A1:U1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3645,7 +3654,7 @@
     <col min="1" max="1" width="35.19921875" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
     <col min="3" max="3" width="35.3984375" customWidth="1"/>
-    <col min="4" max="4" width="71.3984375" customWidth="1"/>
+    <col min="4" max="4" width="80" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="87.59765625" customWidth="1"/>
   </cols>
@@ -3688,22 +3697,22 @@
     </row>
     <row r="4" spans="1:21" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>219</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>221</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -3723,22 +3732,22 @@
     </row>
     <row r="5" spans="1:21" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -3758,22 +3767,22 @@
     </row>
     <row r="6" spans="1:21" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>191</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -3793,22 +3802,22 @@
     </row>
     <row r="7" spans="1:21" ht="76" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -3828,22 +3837,22 @@
     </row>
     <row r="8" spans="1:21" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>229</v>
-      </c>
       <c r="F8" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -3863,22 +3872,22 @@
     </row>
     <row r="9" spans="1:21" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>216</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>218</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -3898,22 +3907,22 @@
     </row>
     <row r="10" spans="1:21" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>195</v>
-      </c>
       <c r="E10" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -3933,22 +3942,22 @@
     </row>
     <row r="11" spans="1:21" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -3968,19 +3977,19 @@
     </row>
     <row r="12" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -4001,19 +4010,19 @@
     </row>
     <row r="13" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -4034,19 +4043,19 @@
     </row>
     <row r="14" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -4067,22 +4076,22 @@
     </row>
     <row r="15" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -4102,19 +4111,19 @@
     </row>
     <row r="16" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>179</v>
-      </c>
       <c r="C16" s="8" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="2"/>
@@ -4135,19 +4144,19 @@
     </row>
     <row r="17" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="2"/>
@@ -4168,19 +4177,19 @@
     </row>
     <row r="18" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>253</v>
-      </c>
       <c r="E18" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="2"/>
@@ -4201,19 +4210,19 @@
     </row>
     <row r="19" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>254</v>
-      </c>
       <c r="E19" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="2"/>
@@ -4232,18 +4241,22 @@
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
     </row>
-    <row r="20" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="2"/>
+        <v>251</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>190</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -4261,20 +4274,22 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
     </row>
-    <row r="21" spans="1:21" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>271</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>190</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -4292,20 +4307,22 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
     </row>
-    <row r="22" spans="1:21" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>236</v>
+        <v>169</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>255</v>
+        <v>173</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>273</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>191</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -4325,13 +4342,13 @@
     </row>
     <row r="23" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>236</v>
+        <v>169</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
+        <v>150</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -4352,13 +4369,13 @@
     </row>
     <row r="24" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="9"/>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -4379,15 +4396,23 @@
     </row>
     <row r="25" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+        <v>259</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>268</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -4406,15 +4431,23 @@
     </row>
     <row r="26" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+        <v>260</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>269</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -4433,20 +4466,14 @@
     </row>
     <row r="27" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>1</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -4466,20 +4493,14 @@
     </row>
     <row r="28" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>1</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -4499,10 +4520,10 @@
     </row>
     <row r="29" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -4526,10 +4547,10 @@
     </row>
     <row r="30" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -4553,10 +4574,10 @@
     </row>
     <row r="31" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -4580,10 +4601,10 @@
     </row>
     <row r="32" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -4607,10 +4628,10 @@
     </row>
     <row r="33" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -4633,12 +4654,8 @@
       <c r="U33" s="2"/>
     </row>
     <row r="34" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>183</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -4660,12 +4677,8 @@
       <c r="U34" s="2"/>
     </row>
     <row r="35" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>186</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -4986,50 +4999,50 @@
       <c r="U48" s="2"/>
     </row>
     <row r="49" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
     </row>
     <row r="50" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="2"/>
-      <c r="U50" s="2"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
     </row>
     <row r="51" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
@@ -5422,7 +5435,7 @@
       <c r="T67" s="3"/>
       <c r="U67" s="3"/>
     </row>
-    <row r="68" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -5445,7 +5458,7 @@
       <c r="T68" s="3"/>
       <c r="U68" s="3"/>
     </row>
-    <row r="69" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -5468,52 +5481,8 @@
       <c r="T69" s="3"/>
       <c r="U69" s="3"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-      <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
-      <c r="N70" s="3"/>
-      <c r="O70" s="3"/>
-      <c r="P70" s="3"/>
-      <c r="Q70" s="3"/>
-      <c r="R70" s="3"/>
-      <c r="S70" s="3"/>
-      <c r="T70" s="3"/>
-      <c r="U70" s="3"/>
-    </row>
-    <row r="71" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
-      <c r="M71" s="3"/>
-      <c r="N71" s="3"/>
-      <c r="O71" s="3"/>
-      <c r="P71" s="3"/>
-      <c r="Q71" s="3"/>
-      <c r="R71" s="3"/>
-      <c r="S71" s="3"/>
-      <c r="T71" s="3"/>
-      <c r="U71" s="3"/>
-    </row>
+    <row r="70" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="72" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="73" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6459,8 +6428,6 @@
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:F2"/>
@@ -8532,7 +8499,7 @@
     </row>
     <row r="2" spans="1:18" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -8540,30 +8507,30 @@
     </row>
     <row r="3" spans="1:18" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="14" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -8582,16 +8549,16 @@
     </row>
     <row r="5" spans="1:18" s="16" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>197</v>
-      </c>
       <c r="C5" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>200</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -8610,16 +8577,16 @@
     </row>
     <row r="6" spans="1:18" s="16" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="9" t="s">
         <v>209</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>210</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -8638,16 +8605,16 @@
     </row>
     <row r="7" spans="1:18" s="16" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>213</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>214</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -8666,16 +8633,16 @@
     </row>
     <row r="8" spans="1:18" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -10543,14 +10510,14 @@
   </sheetPr>
   <dimension ref="A1:S999"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.59765625" customWidth="1"/>
-    <col min="2" max="2" width="44.59765625" customWidth="1"/>
+    <col min="2" max="2" width="56.796875" customWidth="1"/>
     <col min="3" max="3" width="96" customWidth="1"/>
     <col min="4" max="4" width="38.796875" customWidth="1"/>
     <col min="5" max="5" width="45.59765625" customWidth="1"/>
@@ -10591,16 +10558,16 @@
         <v>45124</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>165</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -10622,16 +10589,16 @@
         <v>45134</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>231</v>
+        <v>265</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -10649,11 +10616,21 @@
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="12">
+        <v>45193</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>222</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>

</xml_diff>

<commit_message>
add information on AWOL tool and associated observations and populations from initial research
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/health-ai-performance/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EAFDF4-0B66-D04D-982E-F1DE33250D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A992B6-0F74-794C-A504-9922A7C42B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="290">
   <si>
     <t>Text</t>
   </si>
@@ -484,9 +484,6 @@
     <t>Person responsible for changes</t>
   </si>
   <si>
-    <t>This data dictionary is intended to document the dataset(s) accessible at [internal use only]</t>
-  </si>
-  <si>
     <t>Ad hoc</t>
   </si>
   <si>
@@ -712,9 +709,6 @@
     <t>Algorithm developer</t>
   </si>
   <si>
-    <t>The company, organization, or individual who developed the algorithm</t>
-  </si>
-  <si>
     <t>Is FDA authorized</t>
   </si>
   <si>
@@ -862,7 +856,58 @@
     <t>A unique ID for each metric reported for each algorithm</t>
   </si>
   <si>
-    <t>The data dictionary was last updated on September 24, 2023</t>
+    <t>The company, organization, or individual who developed the algorithm. In the case that a group of academic researchers co-designed that algorithm, the developer will be identified as "Academic researchers" and the first author of the original publication (e.g., "Academic researchers (Douglas et al)")</t>
+  </si>
+  <si>
+    <t>Added additional definitions</t>
+  </si>
+  <si>
+    <t>The data dictionary was last updated on September 25, 2023</t>
+  </si>
+  <si>
+    <t>This data dictionary is intended to document the dataset(s) accessible at https://github.com/seaneff/health-ai-performance</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>The country that patients were recruited from and/or in which data were generated. If multiple countries, "Multiple countries"</t>
+  </si>
+  <si>
+    <t>Sample type</t>
+  </si>
+  <si>
+    <t>The type of sample based on which metrics were calculated. One of: development, validation, or real-world use</t>
+  </si>
+  <si>
+    <t>See definitions tab for definitions of each value</t>
+  </si>
+  <si>
+    <t>development</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>real-world use</t>
+  </si>
+  <si>
+    <t>Data used directly as part of model training (e.g., predictive performance of training dataset).</t>
+  </si>
+  <si>
+    <t>Data not used directly as part of model training (e.g., predictive performance of testing dataset), but collected and analyzed either retrospectively or outside of the context of the algorithm being actively integrated into ongoing clinical care.</t>
+  </si>
+  <si>
+    <t>Data from integration of the algorithm into existing clinical workflows, including real-world timing and deployments and interactions with physician decision-making</t>
   </si>
 </sst>
 </file>
@@ -1314,7 +1359,7 @@
   <dimension ref="A1:V1005"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1334,7 +1379,7 @@
     </row>
     <row r="2" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>148</v>
+        <v>275</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -1382,19 +1427,19 @@
     </row>
     <row r="7" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>167</v>
-      </c>
       <c r="D7" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1416,19 +1461,19 @@
     </row>
     <row r="8" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>203</v>
-      </c>
       <c r="D8" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1450,19 +1495,19 @@
     </row>
     <row r="9" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>205</v>
-      </c>
       <c r="D9" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1484,19 +1529,19 @@
     </row>
     <row r="10" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>234</v>
-      </c>
       <c r="D10" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1518,19 +1563,19 @@
     </row>
     <row r="11" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>171</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>172</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -3643,10 +3688,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U1016"/>
+  <dimension ref="A1:U1019"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3654,7 +3699,7 @@
     <col min="1" max="1" width="35.19921875" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
     <col min="3" max="3" width="35.3984375" customWidth="1"/>
-    <col min="4" max="4" width="80" customWidth="1"/>
+    <col min="4" max="4" width="88.19921875" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="87.59765625" customWidth="1"/>
   </cols>
@@ -3697,22 +3742,22 @@
     </row>
     <row r="4" spans="1:21" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -3732,22 +3777,22 @@
     </row>
     <row r="5" spans="1:21" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>221</v>
-      </c>
       <c r="E5" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -3767,22 +3812,22 @@
     </row>
     <row r="6" spans="1:21" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>190</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -3802,22 +3847,22 @@
     </row>
     <row r="7" spans="1:21" ht="76" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>224</v>
+        <v>272</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -3837,22 +3882,22 @@
     </row>
     <row r="8" spans="1:21" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>227</v>
-      </c>
       <c r="F8" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -3872,22 +3917,22 @@
     </row>
     <row r="9" spans="1:21" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>216</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -3907,22 +3952,22 @@
     </row>
     <row r="10" spans="1:21" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>194</v>
-      </c>
       <c r="E10" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -3942,22 +3987,22 @@
     </row>
     <row r="11" spans="1:21" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>229</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -3977,19 +4022,19 @@
     </row>
     <row r="12" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>237</v>
-      </c>
       <c r="E12" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -4010,19 +4055,19 @@
     </row>
     <row r="13" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>238</v>
-      </c>
       <c r="E13" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -4043,19 +4088,19 @@
     </row>
     <row r="14" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -4076,22 +4121,22 @@
     </row>
     <row r="15" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>229</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -4111,19 +4156,19 @@
     </row>
     <row r="16" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>178</v>
-      </c>
       <c r="C16" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="2"/>
@@ -4144,19 +4189,19 @@
     </row>
     <row r="17" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="2"/>
@@ -4177,19 +4222,19 @@
     </row>
     <row r="18" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="2"/>
@@ -4210,19 +4255,19 @@
     </row>
     <row r="19" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="2"/>
@@ -4243,19 +4288,19 @@
     </row>
     <row r="20" spans="1:21" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>253</v>
-      </c>
       <c r="E20" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -4276,19 +4321,19 @@
     </row>
     <row r="21" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -4309,19 +4354,19 @@
     </row>
     <row r="22" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -4342,10 +4387,10 @@
     </row>
     <row r="23" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -4369,10 +4414,10 @@
     </row>
     <row r="24" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -4396,23 +4441,15 @@
     </row>
     <row r="25" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>268</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -4431,23 +4468,15 @@
     </row>
     <row r="26" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>269</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -4466,15 +4495,23 @@
     </row>
     <row r="27" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+        <v>277</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>283</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -4493,15 +4530,23 @@
     </row>
     <row r="28" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+        <v>257</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>266</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -4520,15 +4565,23 @@
     </row>
     <row r="29" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+        <v>258</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>267</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -4547,15 +4600,21 @@
     </row>
     <row r="30" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+        <v>278</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F30" s="9"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -4574,10 +4633,10 @@
     </row>
     <row r="31" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -4601,7 +4660,7 @@
     </row>
     <row r="32" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>182</v>
@@ -4628,10 +4687,10 @@
     </row>
     <row r="33" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -4654,8 +4713,12 @@
       <c r="U33" s="2"/>
     </row>
     <row r="34" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="A34" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -4677,8 +4740,12 @@
       <c r="U34" s="2"/>
     </row>
     <row r="35" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="A35" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>181</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -4700,8 +4767,12 @@
       <c r="U35" s="2"/>
     </row>
     <row r="36" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+      <c r="A36" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>184</v>
+      </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -4999,73 +5070,73 @@
       <c r="U48" s="2"/>
     </row>
     <row r="49" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
     </row>
     <row r="50" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
     </row>
     <row r="51" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
     </row>
     <row r="52" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
@@ -5435,7 +5506,7 @@
       <c r="T67" s="3"/>
       <c r="U67" s="3"/>
     </row>
-    <row r="68" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -5458,7 +5529,7 @@
       <c r="T68" s="3"/>
       <c r="U68" s="3"/>
     </row>
-    <row r="69" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -5481,9 +5552,75 @@
       <c r="T69" s="3"/>
       <c r="U69" s="3"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+    </row>
+    <row r="71" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3"/>
+      <c r="U71" s="3"/>
+    </row>
+    <row r="72" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="P72" s="3"/>
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="3"/>
+      <c r="T72" s="3"/>
+      <c r="U72" s="3"/>
+    </row>
     <row r="73" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="75" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6428,6 +6565,9 @@
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:F2"/>
@@ -6446,15 +6586,15 @@
   <dimension ref="A1:S999"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.19921875" customWidth="1"/>
-    <col min="2" max="2" width="36.59765625" customWidth="1"/>
-    <col min="3" max="3" width="38.59765625" customWidth="1"/>
-    <col min="4" max="4" width="48.796875" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="27.796875" customWidth="1"/>
+    <col min="4" max="4" width="119.3984375" customWidth="1"/>
     <col min="5" max="5" width="57.59765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6489,10 +6629,18 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>287</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -6509,11 +6657,19 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
     </row>
-    <row r="5" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+    <row r="5" spans="1:19" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>288</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -6531,10 +6687,18 @@
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>289</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -8499,7 +8663,7 @@
     </row>
     <row r="2" spans="1:18" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -8507,30 +8671,30 @@
     </row>
     <row r="3" spans="1:18" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>156</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="14" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>162</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -8549,16 +8713,16 @@
     </row>
     <row r="5" spans="1:18" s="16" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>196</v>
-      </c>
       <c r="C5" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>198</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>199</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -8577,16 +8741,16 @@
     </row>
     <row r="6" spans="1:18" s="16" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="9" t="s">
         <v>208</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>209</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -8605,16 +8769,16 @@
     </row>
     <row r="7" spans="1:18" s="16" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>213</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -8633,16 +8797,16 @@
     </row>
     <row r="8" spans="1:18" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="D8" s="9" t="s">
         <v>256</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>258</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -10511,7 +10675,7 @@
   <dimension ref="A1:S999"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10558,16 +10722,16 @@
         <v>45124</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>164</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -10589,16 +10753,16 @@
         <v>45134</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -10620,16 +10784,16 @@
         <v>45193</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -10647,8 +10811,12 @@
       <c r="S6" s="2"/>
     </row>
     <row r="7" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
+      <c r="A7" s="12">
+        <v>45194</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>273</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>